<commit_message>
updated task 5 place orders
</commit_message>
<xml_diff>
--- a/Test_Data/user_credentials.xlsx
+++ b/Test_Data/user_credentials.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0599</t>
+          <t>2f3c</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -473,7 +473,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>26f8</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4a53</t>
+          <t>c046</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -507,7 +507,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>de36</t>
+          <t>1176</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0599</t>
+          <t>2f3c</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -567,7 +567,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>26f8</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -579,7 +579,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4a53</t>
+          <t>c046</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -591,7 +591,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>de36</t>
+          <t>1176</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -644,7 +644,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3f8f</t>
+          <t>3e00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -666,7 +666,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>869f</t>
+          <t>08b2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>e702</t>
+          <t>568f</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>936a</t>
+          <t>cc8b</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -732,7 +732,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4c06</t>
+          <t>d499</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -754,7 +754,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>e35b</t>
+          <t>7959</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -784,7 +784,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +823,11 @@
           <t>Total Price</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Order Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -851,6 +856,11 @@
       <c r="F2" t="n">
         <v>59.98</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -879,6 +889,11 @@
       <c r="F3" t="n">
         <v>9.99</v>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -906,6 +921,11 @@
       </c>
       <c r="F4" t="n">
         <v>29.99</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>